<commit_message>
Unity test cases are updated for eeprom device
</commit_message>
<xml_diff>
--- a/firmware/ec/test/suites/Doc/TestCaseList.xlsx
+++ b/firmware/ec/test/suites/Doc/TestCaseList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ltc4274" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="312">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -852,10 +852,16 @@
     <t xml:space="preserve">static  i2c_eeprom_write(void)</t>
   </si>
   <si>
+    <t xml:space="preserve">Function is static. Can not call from outside the file. It is covered as part of eeprom_write.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Static function</t>
   </si>
   <si>
     <t xml:space="preserve">static  i2c_eeprom_read(void)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function is static. Can not call from outside the file. It is covered as part of eeprom_read.</t>
   </si>
   <si>
     <t xml:space="preserve">test_eeprom_disable_write(void)</t>
@@ -899,21 +905,10 @@
     <t xml:space="preserve"> test_eeprom_read_device_info_record(void)</t>
   </si>
   <si>
-    <t xml:space="preserve">Initialize rominfo to 0xff. Set register 0x0A01 to 4153.
-initialize a recordno to 1. char *deviceinfo = (char *) malloc(10); 
-define a cfg c1_dev with i2c_dev,pin_wp,type,ss=0  
-Pass the values to eeprom_read_device_info_record() and check for case number if it returns 5 its successs else failure.
-Repeate the steps for other cases with ss=7 and ss=8 respectively</t>
+    <t xml:space="preserve">Function is only stack holder in the code. No UT is required for now.</t>
   </si>
   <si>
     <t xml:space="preserve">test_eeprom_write_device_info_record(void)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initialize a recordno to 1. also initialize a 
- char *deviceinfo = (char *) malloc(10);
-and a memset(deviceinfo,0,10) now copy a string  SA to deviceinfo
-define a cfg d1_dev with i2c_dev,pin_wp,type,ss=0 now write the vaues to the eeprom_write_device_info_record() and check if u get the hex values of SA as 0x4153.
-  Repeate the steps for other cases with ss=7 and ss=8 respectively</t>
   </si>
   <si>
     <t xml:space="preserve">test_static void pwr_update_source_info</t>
@@ -2156,7 +2151,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2172,7 +2167,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
@@ -2184,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,7 +2190,7 @@
         <v>170</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
@@ -2210,7 +2205,7 @@
         <v>198</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
@@ -2222,10 +2217,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
@@ -2237,10 +2232,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -2252,10 +2247,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -2267,10 +2262,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -2282,10 +2277,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -2297,10 +2292,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
@@ -2312,10 +2307,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>9</v>
@@ -2327,10 +2322,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>9</v>
@@ -2342,10 +2337,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
@@ -4157,8 +4152,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4646,17 +4641,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4697,13 +4692,13 @@
         <v>240</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="80.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>2</v>
       </c>
@@ -4718,7 +4713,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="73.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>3</v>
       </c>
@@ -4733,7 +4728,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="73.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>4</v>
       </c>
@@ -4741,30 +4736,30 @@
         <v>246</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>247</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="73.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="130" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4772,16 +4767,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="143" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4789,69 +4784,69 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="63" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="144" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="106.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="106.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>262</v>
@@ -4863,13 +4858,7 @@
     </row>
     <row r="13" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E12">
-    <filterColumn colId="3">
-      <customFilters and="true">
-        <customFilter operator="equal" val="No"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E12"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4928,7 +4917,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>39</v>
@@ -4937,7 +4926,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4945,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>39</v>
@@ -4954,7 +4943,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4962,7 +4951,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>39</v>
@@ -4971,7 +4960,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4979,7 +4968,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>39</v>
@@ -4988,7 +4977,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4996,7 +4985,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>39</v>
@@ -5005,7 +4994,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5013,7 +5002,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>39</v>
@@ -5022,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5030,7 +5019,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>39</v>
@@ -5039,7 +5028,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5047,7 +5036,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>39</v>
@@ -5056,7 +5045,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5064,7 +5053,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>39</v>
@@ -5073,7 +5062,7 @@
         <v>208</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5081,7 +5070,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>39</v>
@@ -5090,7 +5079,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="409.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5098,10 +5087,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
@@ -5139,7 +5128,7 @@
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="4.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="41.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16"/>
@@ -5168,10 +5157,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -5183,10 +5172,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
@@ -5198,10 +5187,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -5213,10 +5202,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
@@ -5228,10 +5217,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
@@ -5243,10 +5232,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Unit test case for ocmp_ina226
</commit_message>
<xml_diff>
--- a/firmware/ec/test/suites/Doc/TestCaseList.xlsx
+++ b/firmware/ec/test/suites/Doc/TestCaseList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ltc4274" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,9 @@
     <sheet name="eeprom" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="PowerSource" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="ltc4275" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="ocmp_powersource" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="ocmp_ltc4015" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="ocmp_powersource" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="ocmp_ina226" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">adt7481!$A$1:$F$37</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="367">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -1019,6 +1021,490 @@
     <t xml:space="preserve">Remark</t>
   </si>
   <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set pin with actual value as 
+    LTC4015_GpioConfig[0x05] = 0;
+Call the probe function using LTC4015_fxnTable 
+Check the return of this function is POST_DEV_FOUND.
+Also check for the gpio configuration s done for pin.
+Now repet this process with wrong bus/slave_address and check that function is returning POST_DEV_MISSING value.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set alert configuration as required. 
+Call the cb_init function using LTC4015_fxnTable 
+Check the return of this function is POST_DEV_FOUND.
+Also check that default configuration is set for all config params.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_battery_voltage_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_status function using LTC4015_fxnTable
+Check for the return value as well as beffer value.
+Repet this process for differt values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_battery_current_get_status</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_status function using LTC4015_fxnTable
+Check for the return value as well as beffer value.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Repet this process for differt values.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_system_voltage_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_input_voltage_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_input_current_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_dia_temerature_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_icharge_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_vcharge_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_invalid_param_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_status function using LTC4015_fxnTable
+Check for the return value as well as beffer value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_battery_voltage_low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_config function using LTC4015_fxnTable
+Check for the return value as well as beffer value.
+Repet this process for different config values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_battery_voltage_high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_battery_current_low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_input_voltage_low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_input_current_high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_input_current_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_icharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_vcharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_dia_temperature_high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_get_cfg_invalid_param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_config function using LTC4015_fxnTable
+Check for the return value as well as beffer value.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_battery_voltage_low</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register with some dummy value.
+Call cb_set_config function using LTC4015_fxnTable
+Check for the return value as well as register value.
+Repet this process for differnet config value.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_battery_voltage_high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_battery_current_low</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_input_voltage_low</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_input_current_high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_input_current_limit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_icharge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_vcharge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_dia_temprature_high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4015_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">set_cfg_invalid_param</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4015_alert_handler</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Set register with actual values
+Call the init function using</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">LTC4015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_fxnTable. 
+Check the return of this function is POST_DEV_CFG_DONE.
+Check the alert data for all alerts .
+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Set pin with actual value as 
     PWR_GpioConfig[0x1E] = OCGPIO_CFG_OUTPUT;
     PWR_GpioConfig[0x55] = OCGPIO_CFG_OUTPUT;
@@ -1114,6 +1600,83 @@
 Set the register value according to the paramert.
 Call cb_get_status function using PWRSRC_fxnTable for invalid parameter ID.
 Check for the return value as well as beffer value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set register with actual value as 
+    INA226_regs[0xFF] = 0x2260;
+    INA226_regs[0xFE] = 0x5449;
+Call the probe function using INA226_fxnTable. 
+Check the return of this function is POST_DEV_FOUND.
+Now repet the process with incorrect device ID and mfg ID and check for the POST_DEV_ID_MISMATCH return value.
+Now repet this process with wrong bus/slave_address and check that function is returning POST_DEV_MISSING value.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set registers as 
+    INA226_regs[0x00] = 0x1234;
+    INA226_regs[0x05] = 0x0000; 
+ INA226_regs[0x07] = 0x0320; 
+Call the cb_init function using INA226_fxnTable. 
+Check the return of this function is POST_DEV_FOUND.
+Make sure we've reset the device and calibration register gets initialized.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_get_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_status function using INA226_fxnTable.
+Check for the return value as well as beffer value.
+Repet this process for every status paramer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_get_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register value according to the paramert.
+Call cb_get_config function using INA226_fxnTable.
+Check for the return value as well as beffer value.
+Repet this process for every config paramer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_set_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable to pass into function as buffer.
+Set the register with some dummy value.
+Call cb_set_config function using INA226_fxnTable.
+Check for the return value as well as register value.
+Repet this process for every config paramer.
+Also test for invalid parameter as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intialize the local variable with out of range value to pass into function as buffer.
+Set the register with some dummy value.
+Call cb_set_config function using INA226_fxnTable.
+Check for the return value as well as register value.
+Repet this process for every config paramer.
+Also test for invalid parameter as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ina226_alert_handler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set register with actual values
+Call the init function using INA226_fxnTable. 
+Check the return of this function is POST_DEV_CFG_DONE.
+Check the alert data for all alerts .
+</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1168,6 +1731,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2149,6 +2718,639 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2190,7 +3392,7 @@
         <v>170</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
@@ -2205,7 +3407,7 @@
         <v>198</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>293</v>
+        <v>334</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
@@ -2217,10 +3419,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>295</v>
+        <v>336</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
@@ -2232,10 +3434,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>296</v>
+        <v>337</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>297</v>
+        <v>338</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -2247,10 +3449,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>299</v>
+        <v>340</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -2262,10 +3464,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>300</v>
+        <v>341</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>301</v>
+        <v>342</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -2277,10 +3479,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>302</v>
+        <v>343</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -2292,10 +3494,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
@@ -2307,10 +3509,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>307</v>
+        <v>348</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>9</v>
@@ -2322,10 +3524,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>308</v>
+        <v>349</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>309</v>
+        <v>350</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>9</v>
@@ -2337,10 +3539,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>310</v>
+        <v>351</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>311</v>
+        <v>352</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
@@ -2351,6 +3553,160 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="13"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4152,7 +5508,7 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -4241,146 +5597,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
-      <c r="B9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4646,11 +5863,11 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Unit test for ocmp_ltc4275
</commit_message>
<xml_diff>
--- a/firmware/ec/test/suites/Doc/TestCaseList.xlsx
+++ b/firmware/ec/test/suites/Doc/TestCaseList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="ltc4274" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <sheet name="ocmp_se98a" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="ocmp_ina226" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="ocmp_eeprom" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="ocmp_ltc4275" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">adt7481!$A$1:$F$37</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="387">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -1441,6 +1442,101 @@
 Call CAT24C04_gbc_sid_fxnTable get status with param id 0/1 and the local buffer.
 Check the value of local but is coming as expected or not.</t>
   </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4275_init()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set registers as:  
+ Gpio_pins[0x60] = 0,
+ Gpio_pins[0x40] = 1.
+Call the init function using LTC4275_fxnTable  and check for all the output set by the function.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4275_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">probe()</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Set pin as LTC4275_GpioPins[0x60] = 1.
+Call the probe function using LTC4275_fxnTable .
+Check for the PDStatus_Info values.
+Now set pin as LTC4275_GpioPins[0x60] = 0.
+Call the probe function using LTC4275_fxnTable.
+Check for the  PDStatus_Info values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">test_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ocmp_ltc4275_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">get_status</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Set a local varibale.
+Call the _get_status function using LTC4275_fxnTable with differen param Id.
+If param id is 1, check for LTC4275_POWERGOOD status.
+If param id is 0, check for classtype.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_ocmp_ltc4275_alert_handler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set register with actual values
+Call the init function using LTC4275_fxnTable. 
+Check the return of this function is POST_DEV_CFG_DONE.
+Check the alert data for all alerts .
+</t>
+  </si>
 </sst>
 </file>
 
@@ -1449,7 +1545,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1494,6 +1590,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3431,7 +3533,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.14"/>
@@ -3547,8 +3649,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3558,7 +3660,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -3702,13 +3804,13 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.55"/>
@@ -3787,6 +3889,115 @@
       </c>
       <c r="C5" s="5" t="s">
         <v>378</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>386</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -6026,7 +6237,7 @@
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="4.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="41.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16"/>

</xml_diff>